<commit_message>
Implement 5-cell professional notebook structure
</commit_message>
<xml_diff>
--- a/Walmart_Business_Analysis_Complete.xlsx
+++ b/Walmart_Business_Analysis_Complete.xlsx
@@ -11,10 +11,11 @@
     <sheet name="Category Performance" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Customer Satisfaction" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Profitability" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Branch Payment Pref" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="High Value Analysis" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Regional Analysis" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Executive Summary" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Time Analysis" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Branch Payment Pref" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="High Value Analysis" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Regional Analysis" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Executive Summary" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1362,6 +1363,95 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>time_period</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>total_transactions</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>total_revenue</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>avg_transaction_value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Afternoon</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>4636</v>
+      </c>
+      <c r="C2" t="n">
+        <v>578817.77</v>
+      </c>
+      <c r="D2" t="n">
+        <v>124.85</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3246</v>
+      </c>
+      <c r="C3" t="n">
+        <v>379401.6</v>
+      </c>
+      <c r="D3" t="n">
+        <v>116.88</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>2087</v>
+      </c>
+      <c r="C4" t="n">
+        <v>251507.01</v>
+      </c>
+      <c r="D4" t="n">
+        <v>120.51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1667,7 +1757,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2030,7 +2120,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2301,13 +2391,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2420,58 +2510,78 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Branch Payment Method Preferences</t>
+          <t>Sales Performance by Time of Day</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Payment infrastructure optimization per location</t>
+          <t>Operational efficiency and staff scheduling optimization</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>7_branch_payment_preferences.csv</t>
+          <t>6_sales_by_time_period.csv</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>High-Value Customer Transaction Analysis</t>
+          <t>Branch Payment Method Preferences</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Premium customer behavior analysis for business growth</t>
+          <t>Payment infrastructure optimization per location</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>8_high_value_transactions.csv</t>
+          <t>7_branch_payment_preferences.csv</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>High-Value Customer Transaction Analysis</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>12</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Premium customer behavior analysis for business growth</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>8_high_value_transactions.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
           <t>Regional Performance Comparison Analysis</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="B9" t="n">
         <v>10</v>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>Market expansion and regional strategy development</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>9_regional_performance_comparison.csv</t>
         </is>

</xml_diff>